<commit_message>
modificacion de archivos 08/02/2019
</commit_message>
<xml_diff>
--- a/Nombre imagenes (Copia en conflicto de DESKTOP-893CF3J 2019-02-01).xlsx
+++ b/Nombre imagenes (Copia en conflicto de DESKTOP-893CF3J 2019-02-01).xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fabrica-01\supaada\Dropbox\.dropbox.cache\2019-01-31\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15630" windowHeight="11145"/>
   </bookViews>
@@ -15,7 +10,7 @@
     <sheet name="Imagenes" sheetId="1" r:id="rId1"/>
     <sheet name="URL" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -344,7 +339,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -379,7 +374,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -556,7 +551,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -567,7 +562,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>